<commit_message>
Occ 2015  edit 1
</commit_message>
<xml_diff>
--- a/Occ_rate_2015_2023.xlsx
+++ b/Occ_rate_2015_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keros\.venv\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B47F6E2-2C7D-4DED-BACE-9C58C22F382D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7844CF97-0A2E-429D-AE7C-A36094D9F73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28545" yWindow="15480" windowWidth="16410" windowHeight="11295" xr2:uid="{F7EB4146-D490-488D-917F-06F799A966E6}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{F7EB4146-D490-488D-917F-06F799A966E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF8E936-6889-4D1F-AD38-0FFFEEC90814}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +528,7 @@
         <v>0.78</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" ref="J3:J53" si="1">(A3+B3+C3+D3+E3+F3+G3+H3+I3)/9</f>
+        <f t="shared" ref="J3:J52" si="1">(A3+B3+C3+D3+E3+F3+G3+H3+I3)/9</f>
         <v>0.81555555555555559</v>
       </c>
       <c r="K3"/>
@@ -2198,40 +2198,6 @@
         <v>0.74888888888888894</v>
       </c>
       <c r="K52"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>0.79</v>
-      </c>
-      <c r="B53" s="1">
-        <v>0.78</v>
-      </c>
-      <c r="C53" s="1">
-        <v>0.82</v>
-      </c>
-      <c r="D53" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0.79</v>
-      </c>
-      <c r="F53" s="1">
-        <v>0.78</v>
-      </c>
-      <c r="G53" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="H53" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="I53" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="J53" s="3">
-        <f t="shared" si="1"/>
-        <v>0.74888888888888894</v>
-      </c>
-      <c r="K53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2452,10 +2418,6 @@
               <xm:f>Sheet1!A52:I52</xm:f>
               <xm:sqref>K52</xm:sqref>
             </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!A53:I53</xm:f>
-              <xm:sqref>K53</xm:sqref>
-            </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
       </x14:sparklineGroups>

</xml_diff>